<commit_message>
Closer on how to solve the problem
</commit_message>
<xml_diff>
--- a/ScenarioCalculator.xlsx
+++ b/ScenarioCalculator.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10FB031-FA9E-4CB8-B649-B352D0F99771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54483944-0BA8-4887-8F48-FEFEF4CA9502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{56217CED-4FC1-4892-A274-CAB13A8BA974}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{56217CED-4FC1-4892-A274-CAB13A8BA974}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$5:$F$49</definedName>
     <definedName name="_tCurrent">Sheet1!$G$3:$G$6</definedName>
     <definedName name="_tScenario">Sheet1!$B$3:$E$7</definedName>
   </definedNames>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="21">
   <si>
     <t>Scenario</t>
   </si>
@@ -83,13 +85,55 @@
   </si>
   <si>
     <t>A,D</t>
+  </si>
+  <si>
+    <t>Nominal</t>
+  </si>
+  <si>
+    <t>E2E</t>
+  </si>
+  <si>
+    <t>Streaming</t>
+  </si>
+  <si>
+    <t>iE2E</t>
+  </si>
+  <si>
+    <t>iNom</t>
+  </si>
+  <si>
+    <t>iStream</t>
+  </si>
+  <si>
+    <t>Typical</t>
+  </si>
+  <si>
+    <t>Extreme</t>
+  </si>
+  <si>
+    <t>Accessory</t>
+  </si>
+  <si>
+    <t>Streaming2</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Wtypical</t>
+  </si>
+  <si>
+    <t>Wextreme</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,16 +141,86 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000099"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -114,18 +228,155 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="10">
+    <cellStyle name="20% - Accent1 2" xfId="9" xr:uid="{2BC3E52E-E329-424F-A2DB-FADA26728F29}"/>
+    <cellStyle name="20% - Accent3 2" xfId="2" xr:uid="{3EAD3B74-547C-417C-A842-8498DCF7608A}"/>
+    <cellStyle name="Comment" xfId="6" xr:uid="{B9FA08FD-3471-4D7D-9E0D-FA24D7CD8C9D}"/>
+    <cellStyle name="Explanatory Text 2" xfId="4" xr:uid="{E1092FDB-B65A-4E63-B5F9-4C40041A7152}"/>
+    <cellStyle name="Heading 1 2" xfId="3" xr:uid="{CD788582-E54C-40BC-A4E7-781480E3C236}"/>
+    <cellStyle name="Heading 2 2" xfId="8" xr:uid="{6DE6B0EE-965E-443E-AC67-C3DDB0D0A318}"/>
+    <cellStyle name="Heading 3 2" xfId="7" xr:uid="{459F3F79-6828-4CB4-B5CF-E5DA336AC396}"/>
+    <cellStyle name="Input 2" xfId="5" xr:uid="{17A33D62-01D2-4B5B-9981-9E58DD73261E}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{14809DE0-748D-40ED-A839-165B00407D24}"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEAEA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <top style="double">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="double">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Biegert Standard" table="0" count="4" xr9:uid="{A6CC9633-40A9-4A30-B81E-42DCEC58198A}">
+      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="totalRow" dxfId="6"/>
+      <tableStyleElement type="firstColumn" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+    </tableStyle>
+    <tableStyle name="Biegert Standard A" pivot="0" count="4" xr9:uid="{93638CB3-BFA6-497F-9859-8BD00F60B78C}">
+      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="totalRow" dxfId="2"/>
+      <tableStyleElement type="firstColumn" dxfId="1"/>
+      <tableStyleElement type="firstRowStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -135,6 +386,36 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3DFC8CC8-B681-46B5-A888-13BBCF0918D9}" name="_tHours" displayName="_tHours" ref="B11:G25" totalsRowShown="0">
+  <autoFilter ref="B11:G25" xr:uid="{3DFC8CC8-B681-46B5-A888-13BBCF0918D9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B12:G25">
+    <sortCondition ref="B11:B25"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B0837AE4-01D9-4682-9142-33209669F896}" name="Scenario"/>
+    <tableColumn id="5" xr3:uid="{FEF9957C-26A5-46A2-8C4C-394213791614}" name="Profile"/>
+    <tableColumn id="6" xr3:uid="{16F27615-E7DF-439B-BFA7-27340121CF0D}" name="Streaming"/>
+    <tableColumn id="2" xr3:uid="{68B3325E-0B99-4CBB-8814-BB4733E39F38}" name="Nominal"/>
+    <tableColumn id="3" xr3:uid="{42C313C3-684B-410D-93CD-3EA67680AE34}" name="E2E"/>
+    <tableColumn id="4" xr3:uid="{C467750C-6A3D-4936-A4FA-698CA2C170D4}" name="Streaming2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{48AECA54-904B-4684-9829-D8EDBC43FED2}" name="_tCur" displayName="_tCur" ref="K11:M14" totalsRowShown="0">
+  <autoFilter ref="K11:M14" xr:uid="{48AECA54-904B-4684-9829-D8EDBC43FED2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{418D190B-E2C5-44F5-AA3F-711872F92FFB}" name="iNom"/>
+    <tableColumn id="2" xr3:uid="{6F2ECD2D-040E-4470-BE63-FBDDFC7EAEA4}" name="iE2E"/>
+    <tableColumn id="3" xr3:uid="{A791471C-31A9-4F3E-8EAA-DFCE4F6439CD}" name="iStream"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD4B868-6795-4819-A53E-3772985205B5}">
   <dimension ref="A2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,4 +948,489 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0C8B2B-C53B-4C0B-AD8C-46E3AE6C3C10}">
+  <dimension ref="B4:U30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="P9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="P10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <v>0.1</v>
+      </c>
+      <c r="L12">
+        <v>0.2</v>
+      </c>
+      <c r="M12">
+        <v>0.3</v>
+      </c>
+      <c r="O12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P12" cm="1">
+        <f t="array" ref="P12">SUMPRODUCT(_xlfn.XLOOKUP($O12&amp;P$9&amp;P$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>1.4</v>
+      </c>
+      <c r="Q12" cm="1">
+        <f t="array" ref="Q12">SUMPRODUCT(_xlfn.XLOOKUP($O12&amp;Q$9&amp;Q$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>-14</v>
+      </c>
+      <c r="R12" cm="1">
+        <f t="array" ref="R12">SUMPRODUCT(_xlfn.XLOOKUP($O12&amp;R$9&amp;R$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>-1.4</v>
+      </c>
+      <c r="S12" cm="1">
+        <f t="array" ref="S12">SUMPRODUCT(_xlfn.XLOOKUP($O12&amp;S$9&amp;S$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>-1.4</v>
+      </c>
+      <c r="T12" cm="1">
+        <f t="array" ref="T12">SUMPRODUCT(_xlfn.XLOOKUP($O12&amp;T$9&amp;T$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>1400</v>
+      </c>
+      <c r="U12" cm="1">
+        <f t="array" ref="U12">SUMPRODUCT(_xlfn.XLOOKUP($O12&amp;U$9&amp;U$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="F13">
+        <v>-2</v>
+      </c>
+      <c r="G13">
+        <v>-3</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="O13" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" cm="1">
+        <f t="array" ref="P13">SUMPRODUCT(_xlfn.XLOOKUP($O13&amp;P$9&amp;P$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>28</v>
+      </c>
+      <c r="Q13" cm="1">
+        <f t="array" ref="Q13">SUMPRODUCT(_xlfn.XLOOKUP($O13&amp;Q$9&amp;Q$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>-280</v>
+      </c>
+      <c r="R13" cm="1">
+        <f t="array" ref="R13">SUMPRODUCT(_xlfn.XLOOKUP($O13&amp;R$9&amp;R$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>-28</v>
+      </c>
+      <c r="S13" cm="1">
+        <f t="array" ref="S13">SUMPRODUCT(_xlfn.XLOOKUP($O13&amp;S$9&amp;S$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>-28</v>
+      </c>
+      <c r="T13" t="e" cm="1">
+        <f t="array" ref="T13">SUMPRODUCT(_xlfn.XLOOKUP($O13&amp;T$9&amp;T$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U13" t="e" cm="1">
+        <f t="array" ref="U13">SUMPRODUCT(_xlfn.XLOOKUP($O13&amp;U$9&amp;U$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>-10</v>
+      </c>
+      <c r="F14">
+        <v>-20</v>
+      </c>
+      <c r="G14">
+        <v>-30</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <v>20</v>
+      </c>
+      <c r="M14">
+        <v>30</v>
+      </c>
+      <c r="O14" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" cm="1">
+        <f t="array" ref="P14">SUMPRODUCT(_xlfn.XLOOKUP($O14&amp;P$9&amp;P$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>420</v>
+      </c>
+      <c r="Q14" cm="1">
+        <f t="array" ref="Q14">SUMPRODUCT(_xlfn.XLOOKUP($O14&amp;Q$9&amp;Q$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>-4200</v>
+      </c>
+      <c r="R14" cm="1">
+        <f t="array" ref="R14">SUMPRODUCT(_xlfn.XLOOKUP($O14&amp;R$9&amp;R$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>-420</v>
+      </c>
+      <c r="S14" cm="1">
+        <f t="array" ref="S14">SUMPRODUCT(_xlfn.XLOOKUP($O14&amp;S$9&amp;S$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>-420</v>
+      </c>
+      <c r="T14" t="e" cm="1">
+        <f t="array" ref="T14">SUMPRODUCT(_xlfn.XLOOKUP($O14&amp;T$9&amp;T$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U14" t="e" cm="1">
+        <f t="array" ref="U14">SUMPRODUCT(_xlfn.XLOOKUP($O14&amp;U$9&amp;U$10,_tHours[[Scenario]:[Scenario]]&amp;_tHours[[Profile]:[Profile]]&amp;_tHours[[Streaming]:[Streaming]],_tHours[[Nominal]:[Streaming2]]),_tCur[#This Row])</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>-1</v>
+      </c>
+      <c r="F15">
+        <v>-2</v>
+      </c>
+      <c r="G15">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16">
+        <v>1000</v>
+      </c>
+      <c r="F16">
+        <v>2000</v>
+      </c>
+      <c r="G16">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>2000</v>
+      </c>
+      <c r="F17">
+        <v>4000</v>
+      </c>
+      <c r="G17">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>-2</v>
+      </c>
+      <c r="F19">
+        <v>-4</v>
+      </c>
+      <c r="G19">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>-20</v>
+      </c>
+      <c r="F20">
+        <v>-40</v>
+      </c>
+      <c r="G20">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>-2</v>
+      </c>
+      <c r="F21">
+        <v>-4</v>
+      </c>
+      <c r="G21">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>-3</v>
+      </c>
+      <c r="F23">
+        <v>-6</v>
+      </c>
+      <c r="G23">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>-30</v>
+      </c>
+      <c r="F24">
+        <v>-60</v>
+      </c>
+      <c r="G24">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>-3</v>
+      </c>
+      <c r="F25">
+        <v>-6</v>
+      </c>
+      <c r="G25">
+        <v>-9</v>
+      </c>
+      <c r="J25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>-10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>